<commit_message>
Adding submission info columns to legacy xlsx export (#1573)
* Adding submission info columns to legacy xlsx export

* Also making tests work
</commit_message>
<xml_diff>
--- a/ozone/tests/examples/art7_rounding_issues.xlsx
+++ b/ozone/tests/examples/art7_rounding_issues.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\edw\projects\ozone\src\ozone\tests\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FD70E1-6AAC-4D59-9F16-6B28B423A66A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFAB7F5E-0F15-4420-9167-627B468E66F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="74">
   <si>
     <t>CntryID</t>
   </si>
@@ -245,6 +245,18 @@
   </si>
   <si>
     <t>NPB</t>
+  </si>
+  <si>
+    <t>ReportingOfficer</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>CreatedByUserEmail</t>
+  </si>
+  <si>
+    <t>secretariat@example.com</t>
   </si>
 </sst>
 </file>
@@ -280,27 +292,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -315,16 +337,7 @@
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -340,18 +353,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DEE233AC-D6E8-436D-A998-AA305F7D179B}" name="Table4" displayName="Table4" ref="A1:AE2" totalsRowShown="0">
-  <autoFilter ref="A1:AE2" xr:uid="{BBA827FF-3408-4520-B936-9A7B51CA9009}"/>
-  <tableColumns count="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DEE233AC-D6E8-436D-A998-AA305F7D179B}" name="Table4" displayName="Table4" ref="A1:AH2" totalsRowShown="0">
+  <autoFilter ref="A1:AH2" xr:uid="{BBA827FF-3408-4520-B936-9A7B51CA9009}"/>
+  <tableColumns count="34">
     <tableColumn id="1" xr3:uid="{EF6F9FB5-ECC5-4EA0-94F8-0659130D77CE}" name="CntryID"/>
-    <tableColumn id="2" xr3:uid="{5E4F564A-9C22-42A2-9294-0123B6E6582D}" name="PeriodID" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{5E4F564A-9C22-42A2-9294-0123B6E6582D}" name="PeriodID" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{E1B07C0F-0BA1-435A-9DF6-1B76B3290C22}" name="DataID"/>
     <tableColumn id="4" xr3:uid="{D810CB4D-5AF4-478E-971E-264B400A7632}" name="Imported"/>
     <tableColumn id="5" xr3:uid="{610400EB-905D-4ED7-807A-C8B8B60F44C4}" name="Exported"/>
     <tableColumn id="6" xr3:uid="{7247FA91-F44D-4639-B80A-5C68EF3E8BA1}" name="Produced"/>
     <tableColumn id="7" xr3:uid="{660EEA51-2C02-48F5-B328-AC2C21289E5F}" name="Destroyed"/>
     <tableColumn id="8" xr3:uid="{506B72B3-3334-4E82-8D35-B0BE322FA98E}" name="NonPartyTrade"/>
-    <tableColumn id="9" xr3:uid="{F1C84320-D2FC-49B5-87E3-5F652AD4391C}" name="DateReported" dataDxfId="11"/>
+    <tableColumn id="9" xr3:uid="{F1C84320-D2FC-49B5-87E3-5F652AD4391C}" name="DateReported" dataDxfId="10"/>
     <tableColumn id="10" xr3:uid="{F5409D96-0EC2-45CA-8501-3D6986DB61E0}" name="AI_ComplRep"/>
     <tableColumn id="11" xr3:uid="{E2207AB4-BB9E-4634-A098-F173A2BF63AC}" name="AII_ComplRep"/>
     <tableColumn id="12" xr3:uid="{80FEFC13-11EE-4583-83E0-337EFCF0318E}" name="BI_ComplRep"/>
@@ -374,6 +387,9 @@
     <tableColumn id="29" xr3:uid="{CCDD547C-0A94-41AE-B1A4-FE4D054910F7}" name="TS"/>
     <tableColumn id="30" xr3:uid="{AF4212CD-4E84-44A9-92D4-377C99675481}" name="Emitted"/>
     <tableColumn id="31" xr3:uid="{9349C437-1462-4EFA-ACD5-BB552CFB7F7D}" name="HFCDateReported"/>
+    <tableColumn id="32" xr3:uid="{8FE86A3D-4BF7-435C-A65A-F87794FFA4F1}" name="ReportingOfficer"/>
+    <tableColumn id="33" xr3:uid="{B57D8514-38C8-4FE1-89AE-277C14671408}" name="Email"/>
+    <tableColumn id="34" xr3:uid="{6C30FA09-41E4-48FF-B1E1-610CB319BCE1}" name="CreatedByUserEmail" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -384,7 +400,7 @@
   <autoFilter ref="A1:R2" xr:uid="{869B2A63-4BCE-423B-BA0F-F990197989D5}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{49B8BBB7-643D-4DEE-9090-6A6872279FAF}" name="CntryID"/>
-    <tableColumn id="2" xr3:uid="{36A76A9C-1377-4051-BBEF-76F8F4A6D00B}" name="PeriodID" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{36A76A9C-1377-4051-BBEF-76F8F4A6D00B}" name="PeriodID" dataDxfId="9"/>
     <tableColumn id="3" xr3:uid="{72595D92-562A-4BC3-B0D8-0C6A0EC9D233}" name="SubstID"/>
     <tableColumn id="4" xr3:uid="{E23AF18F-8FC2-494C-B797-20E8CC133E18}" name="DataID"/>
     <tableColumn id="5" xr3:uid="{AAF3755B-0C16-47E2-BC80-DBFD9B5A1495}" name="ImpNew"/>
@@ -411,7 +427,7 @@
   <autoFilter ref="A1:S2" xr:uid="{B883BA67-43CA-4E5A-A0BE-B429937A0C73}"/>
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{E3E8AEAE-713E-40AE-820D-0A680230FE2A}" name="CntryID"/>
-    <tableColumn id="2" xr3:uid="{B31E4F59-CED0-43C4-82EF-64815C25FC47}" name="PeriodID" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{B31E4F59-CED0-43C4-82EF-64815C25FC47}" name="PeriodID" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{0444F339-F60F-432E-8935-04AA083A1934}" name="SubstID"/>
     <tableColumn id="4" xr3:uid="{7C4BCB8F-8B7F-4982-95C1-A4236AB9E972}" name="OrgCntryID"/>
     <tableColumn id="5" xr3:uid="{2E9A8C21-3F46-49CF-A907-F45BF217AD61}" name="DataID"/>
@@ -439,7 +455,7 @@
   <autoFilter ref="A1:R2" xr:uid="{F03984B7-59FF-4C12-855B-9771CB1523C5}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{D110F4BE-4B0C-4F89-8225-C42788DB850E}" name="CntryID"/>
-    <tableColumn id="2" xr3:uid="{52A62331-69D7-41F2-B39F-9FDB492317C1}" name="PeriodID" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{52A62331-69D7-41F2-B39F-9FDB492317C1}" name="PeriodID" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{CB67B117-A423-49FB-B00D-A2AB05F5E6BF}" name="SubstID"/>
     <tableColumn id="4" xr3:uid="{AA4D12AF-B025-4BC5-B13B-D6C6C9922091}" name="DestCntryID"/>
     <tableColumn id="5" xr3:uid="{2E516163-61AE-4394-AD11-0A25B5A4AED4}" name="DataID"/>
@@ -452,7 +468,7 @@
     <tableColumn id="12" xr3:uid="{6686A83D-E688-4A2E-8EA3-06AE3FD8E200}" name="ExpPolyol"/>
     <tableColumn id="13" xr3:uid="{42AA45DB-6E5F-4231-9263-D2B31F03A4C0}" name="UserCreate"/>
     <tableColumn id="14" xr3:uid="{36D7B9BE-1AAE-4A95-80E5-15FE065BE04E}" name="UserUpdate"/>
-    <tableColumn id="15" xr3:uid="{C054E278-536F-4373-A98D-CAAF08EE83E7}" name="DateCreate" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{C054E278-536F-4373-A98D-CAAF08EE83E7}" name="DateCreate" dataDxfId="6"/>
     <tableColumn id="16" xr3:uid="{722F79BA-5799-4D55-B3DA-B8E7DD3C93BC}" name="DateUpdate"/>
     <tableColumn id="17" xr3:uid="{2C2BF08D-8C3B-4F72-9BA3-F66FDFF76411}" name="Remark"/>
     <tableColumn id="18" xr3:uid="{B7201A53-3FED-4CF2-9533-DD00E4C8F8ED}" name="TS"/>
@@ -466,7 +482,7 @@
   <autoFilter ref="A1:R2" xr:uid="{586F108C-802D-4668-BB80-E4908C473745}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{9902BA22-95CD-4588-9661-59EAEB7DBCE0}" name="CntryID"/>
-    <tableColumn id="2" xr3:uid="{D3395449-1E18-4B01-98A8-C6503DD69095}" name="PeriodID" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{D3395449-1E18-4B01-98A8-C6503DD69095}" name="PeriodID" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{4CD86C0F-50C9-4EAF-870B-963A0E248062}" name="SubstID"/>
     <tableColumn id="4" xr3:uid="{BEE6A254-A090-43F6-828A-EEBB23A9122B}" name="DataID"/>
     <tableColumn id="5" xr3:uid="{3E323866-5157-4C7E-B21B-E3873D1B7145}" name="ProdAllNew"/>
@@ -478,7 +494,7 @@
     <tableColumn id="11" xr3:uid="{F8788740-4212-4BA6-AC55-7001C231552F}" name="ProdProcAgent"/>
     <tableColumn id="12" xr3:uid="{0360D490-6F3E-4334-BF4D-0DEC4C4903FA}" name="UserCreate"/>
     <tableColumn id="13" xr3:uid="{36C79943-426D-42FB-A6C7-46008B5C141B}" name="UserUpdate"/>
-    <tableColumn id="14" xr3:uid="{53F81C4C-FBF6-4262-B929-F80EE43EDC49}" name="DateCreate" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{53F81C4C-FBF6-4262-B929-F80EE43EDC49}" name="DateCreate" dataDxfId="4"/>
     <tableColumn id="15" xr3:uid="{561FE55D-4EF0-44A8-8EF7-B03584634BFA}" name="DateUpdate"/>
     <tableColumn id="16" xr3:uid="{C94062BF-7E9F-4C18-B53B-087D8C3D829D}" name="Remark"/>
     <tableColumn id="17" xr3:uid="{4DC06A45-996C-422C-AD8E-36A9BE2494FA}" name="TS"/>
@@ -513,7 +529,7 @@
   <autoFilter ref="A1:M2" xr:uid="{C16EFE9E-5B41-440A-BD2A-8CE0967FC9D5}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{5167AEED-CB40-4F19-818C-FA9F995652F7}" name="CntryID"/>
-    <tableColumn id="2" xr3:uid="{759AFCB5-8E28-4A9B-B4E0-F67EE8E8161C}" name="PeriodID" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{759AFCB5-8E28-4A9B-B4E0-F67EE8E8161C}" name="PeriodID" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{F7A61370-DE94-46AD-858D-A7FE44995204}" name="SubstID"/>
     <tableColumn id="4" xr3:uid="{5BFAD8E9-4A35-4EA6-8BE1-CC1CCF09F5D7}" name="DataID"/>
     <tableColumn id="5" xr3:uid="{1D68633C-9193-4A20-AD22-A487F5E5CE1F}" name="SrcDestCntryID"/>
@@ -521,7 +537,7 @@
     <tableColumn id="7" xr3:uid="{5815E7CA-6DF9-4B51-A014-A78BC1345C3E}" name="Export"/>
     <tableColumn id="8" xr3:uid="{39A661C2-BFEA-45FC-85A2-E6F600DC687C}" name="UserCreate"/>
     <tableColumn id="9" xr3:uid="{95AAE089-739F-4DE1-9FFE-86D05D022241}" name="UserUpdate"/>
-    <tableColumn id="10" xr3:uid="{88ED29BF-DD26-4FFD-99AB-0505E4416DE0}" name="DateCreate" dataDxfId="8"/>
+    <tableColumn id="10" xr3:uid="{88ED29BF-DD26-4FFD-99AB-0505E4416DE0}" name="DateCreate" dataDxfId="2"/>
     <tableColumn id="11" xr3:uid="{CB05999B-5C50-4963-A750-D7C0E38D3286}" name="DateUpdate"/>
     <tableColumn id="12" xr3:uid="{8A1C212C-8233-4457-BC3E-5ADB42E66348}" name="Remark"/>
     <tableColumn id="13" xr3:uid="{6D772751-6186-4071-938D-7478CBD4606C}" name="TS"/>
@@ -535,7 +551,7 @@
   <autoFilter ref="A1:O2" xr:uid="{7B3EDCB2-32B5-4D26-A862-9D31FABB379B}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{831F65DC-8501-4B6B-ACB7-2BFDC7858965}" name="CntryID"/>
-    <tableColumn id="2" xr3:uid="{3B3F2365-A27B-4206-BD4C-769D1EA80F01}" name="PeriodID" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{3B3F2365-A27B-4206-BD4C-769D1EA80F01}" name="PeriodID" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{8C88FE18-A913-4CC8-9228-9B63C4F0AA43}" name="SubstID"/>
     <tableColumn id="4" xr3:uid="{E07F18BD-60E9-40FE-9A03-04229565A5AD}" name="DataID"/>
     <tableColumn id="5" xr3:uid="{0267BBF2-219B-4F99-8F38-4316BB54EB98}" name="SrcDestCntryID"/>
@@ -545,7 +561,7 @@
     <tableColumn id="9" xr3:uid="{7E3D9F8E-1D66-404E-9E4E-A7F603D740F2}" name="NPTExpRecov"/>
     <tableColumn id="10" xr3:uid="{255D48F7-C317-4640-BB16-9535611B469A}" name="UserCreate"/>
     <tableColumn id="11" xr3:uid="{81867AA5-D6B1-4451-A6A5-C62AA3DF7871}" name="UserUpdate"/>
-    <tableColumn id="12" xr3:uid="{8D929B3A-5D61-4415-A107-23B83AF6C8ED}" name="DateCreate" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{8D929B3A-5D61-4415-A107-23B83AF6C8ED}" name="DateCreate" dataDxfId="0"/>
     <tableColumn id="13" xr3:uid="{2D2F3A8D-736B-49E7-8835-0946AF19974D}" name="DateUpdate"/>
     <tableColumn id="14" xr3:uid="{FF0B1036-E480-48A1-8EF6-6A9F6AC0ECAC}" name="Remark"/>
     <tableColumn id="15" xr3:uid="{40082F20-1D55-416A-A471-267CD622C9CB}" name="TS"/>
@@ -839,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,9 +891,12 @@
     <col min="28" max="28" width="17.5703125" customWidth="1"/>
     <col min="30" max="30" width="10.140625" customWidth="1"/>
     <col min="31" max="31" width="19" customWidth="1"/>
+    <col min="32" max="32" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="21.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -971,8 +990,17 @@
       <c r="AE1" t="s">
         <v>30</v>
       </c>
+      <c r="AF1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -1043,6 +1071,10 @@
         <v>0</v>
       </c>
       <c r="AE2" s="2"/>
+      <c r="AG2" s="4"/>
+      <c r="AH2" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1613,8 +1645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>